<commit_message>
feat: added illustrated message tokens
</commit_message>
<xml_diff>
--- a/spec-tokens.xlsx
+++ b/spec-tokens.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthdb/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garthdb/Spectrum/spectrum-tokens/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1D3CE20-8679-D94D-83D6-67E8BBA2AD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49245AF8-827A-C34E-9BB8-C4C1BFA1BF10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="1820" windowWidth="21360" windowHeight="20520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11180" yWindow="520" windowWidth="36140" windowHeight="21880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
@@ -2424,18 +2424,18 @@
     <t>red-500</t>
   </si>
   <si>
-    <t>#FF9B88 (light)_x000D_
-#D71913 (dark)_x000D_
-#C40706 (darkest)_x000D_
+    <t>#FF9B88 (light)
+#D71913 (dark)
+#C40706 (darkest)
 #D8E1F4 (wireframe)</t>
   </si>
   <si>
     <t>red-600</t>
   </si>
   <si>
-    <t>#FF7C65 (light)_x000D_
-#EA3829 (dark)_x000D_
-#DD2118 (darkest)_x000D_
+    <t>#FF7C65 (light)
+#EA3829 (dark)
+#DD2118 (darkest)
 #CBD7F1 (wireframe)</t>
   </si>
   <si>
@@ -2460,9 +2460,9 @@
     <t>red-900</t>
   </si>
   <si>
-    <t>#D31510 (light)_x000D_
-#FF9581 (dark)_x000D_
-#FF816B (darkest)_x000D_
+    <t>#D31510 (light)
+#FF9581 (dark)
+#FF816B (darkest)
 #9AB1E3 (wireframe)</t>
   </si>
   <si>
@@ -6760,9 +6760,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I185"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B249" sqref="B249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10296,9 +10296,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F2BE219-7E9B-451A-BD2E-F86DF4EBA445}">
   <dimension ref="A1:I362"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A327" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A351" sqref="A351:D351"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A324" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A344" sqref="A344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16116,9 +16116,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8729FF3C-6D27-4452-8072-323C67F98C75}">
   <dimension ref="A1:G232"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19171,7 +19171,7 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -20484,8 +20484,8 @@
   <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A84" sqref="A82:A84"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28466,12 +28466,22 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="8ee4a0ce-e9c8-448f-95e8-0be97c8ae141">
+      <UserInfo>
+        <DisplayName>Erik Holley</DisplayName>
+        <AccountId>66</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Farrell</DisplayName>
+        <AccountId>225</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28672,28 +28682,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="8ee4a0ce-e9c8-448f-95e8-0be97c8ae141">
-      <UserInfo>
-        <DisplayName>Erik Holley</DisplayName>
-        <AccountId>66</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Farrell</DisplayName>
-        <AccountId>225</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3764340F-59F8-4D85-9AA3-1B570AA4ED86}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905EC822-C85D-4815-A526-0083FD207757}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="52308ad5-aa2d-4701-bd11-5edd481a7970"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8ee4a0ce-e9c8-448f-95e8-0be97c8ae141"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28718,18 +28727,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{905EC822-C85D-4815-A526-0083FD207757}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3764340F-59F8-4D85-9AA3-1B570AA4ED86}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="52308ad5-aa2d-4701-bd11-5edd481a7970"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8ee4a0ce-e9c8-448f-95e8-0be97c8ae141"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>